<commit_message>
decrease expected spending a little
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/expected spending.xlsx
+++ b/Modding resources/economy spreadsheets/expected spending.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
   <si>
     <t>adm</t>
   </si>
@@ -521,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D6:V30"/>
+  <dimension ref="D6:V58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,6 +1679,674 @@
         <v>16</v>
       </c>
     </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>2.5</v>
+      </c>
+      <c r="F35">
+        <v>3.5</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="K35">
+        <f>SUM(E35:J35)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36">
+        <v>2.5</v>
+      </c>
+      <c r="F36">
+        <v>3.5</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <v>1.5</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="J36">
+        <v>2.5</v>
+      </c>
+      <c r="K36">
+        <f t="shared" ref="K36:K58" si="8">SUM(E36:J36)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37">
+        <v>1.5</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>2.5</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>2.5</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="J39">
+        <v>1.5</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>2.5</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="8"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>1.5</v>
+      </c>
+      <c r="I42">
+        <v>1.5</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>2.5</v>
+      </c>
+      <c r="J43">
+        <v>2.5</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44">
+        <v>3.5</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <v>2</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="8"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>1.5</v>
+      </c>
+      <c r="H46">
+        <v>1.5</v>
+      </c>
+      <c r="I46">
+        <v>1.5</v>
+      </c>
+      <c r="J46">
+        <v>4</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="8"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47">
+        <v>1.5</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>2.5</v>
+      </c>
+      <c r="H47">
+        <v>2.5</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+      <c r="J47">
+        <v>2.5</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48">
+        <v>3.5</v>
+      </c>
+      <c r="F48">
+        <v>3.5</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
+        <v>2</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>2</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>2.5</v>
+      </c>
+      <c r="J49">
+        <v>2.5</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>2.5</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>2</v>
+      </c>
+      <c r="J50">
+        <v>2.5</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51">
+        <v>1.5</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51">
+        <v>3.5</v>
+      </c>
+      <c r="H51">
+        <v>3</v>
+      </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
+      <c r="J51">
+        <v>2</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52">
+        <v>2.5</v>
+      </c>
+      <c r="F52">
+        <v>1.5</v>
+      </c>
+      <c r="G52">
+        <v>4</v>
+      </c>
+      <c r="H52">
+        <v>2.5</v>
+      </c>
+      <c r="I52">
+        <v>2.5</v>
+      </c>
+      <c r="J52">
+        <v>2</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53">
+        <v>2.5</v>
+      </c>
+      <c r="F53">
+        <v>1.5</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
+      </c>
+      <c r="I53">
+        <v>3</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <v>2.5</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>2.5</v>
+      </c>
+      <c r="I54">
+        <v>2.5</v>
+      </c>
+      <c r="J54">
+        <v>2.5</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55">
+        <v>1.5</v>
+      </c>
+      <c r="F55">
+        <v>4</v>
+      </c>
+      <c r="G55">
+        <v>1.5</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>4</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56">
+        <v>2.5</v>
+      </c>
+      <c r="F56">
+        <v>3.5</v>
+      </c>
+      <c r="G56">
+        <v>1.5</v>
+      </c>
+      <c r="H56">
+        <v>1.5</v>
+      </c>
+      <c r="I56">
+        <v>1.5</v>
+      </c>
+      <c r="J56">
+        <v>4</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="8"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57">
+        <v>2.5</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+      <c r="H57">
+        <v>2</v>
+      </c>
+      <c r="I57">
+        <v>2</v>
+      </c>
+      <c r="J57">
+        <v>3.5</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58">
+        <v>2</v>
+      </c>
+      <c r="J58">
+        <v>2</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>